<commit_message>
Update of the documents
</commit_message>
<xml_diff>
--- a/Historias de Usuario.xlsx
+++ b/Historias de Usuario.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AA0FB9-9D69-4B2A-A6A8-72B03522284D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDAC1B9-19C8-4366-BD81-C5CB57A8D653}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="18">
   <si>
     <t>No. Historia</t>
   </si>
@@ -72,7 +72,10 @@
     <t>Almacenamiento de archivos, qué hacer cuando se llena?</t>
   </si>
   <si>
-    <t>40/80</t>
+    <t>Las evidencias solo se podran ver si perteneces al mismo proyecto que esa evidencia, la excepcion es el administrador de grupo y el super administrador</t>
+  </si>
+  <si>
+    <t>El chat, tiene un bug de resize al borrar</t>
   </si>
 </sst>
 </file>
@@ -104,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,8 +138,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -168,11 +177,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -180,11 +237,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1179,8 +1242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A01F61C9-7A9C-4D17-A094-B2FB3DF79C05}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,7 +1251,7 @@
     <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -1204,7 +1267,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="5">
         <v>1</v>
@@ -1230,17 +1293,17 @@
       <c r="I2" s="5">
         <v>8</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="8">
         <v>1</v>
       </c>
-      <c r="L2">
-        <v>12</v>
-      </c>
-      <c r="M2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L2" s="12">
+        <v>46</v>
+      </c>
+      <c r="M2" s="15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="5">
         <v>9</v>
@@ -1266,14 +1329,14 @@
       <c r="I3" s="5">
         <v>16</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="8">
         <v>8</v>
       </c>
-      <c r="L3" s="8">
-        <v>51</v>
-      </c>
-      <c r="M3">
-        <v>61</v>
+      <c r="L3" s="13">
+        <v>12</v>
+      </c>
+      <c r="M3" s="11">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1302,14 +1365,17 @@
       <c r="I4" s="5">
         <v>24</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="9">
         <v>9</v>
       </c>
-      <c r="L4" s="9">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L4" s="10">
+        <v>51</v>
+      </c>
+      <c r="M4">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="6">
         <v>25</v>
@@ -1335,14 +1401,17 @@
       <c r="I5" s="5">
         <v>32</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="9">
         <v>22</v>
       </c>
-      <c r="L5">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L5" s="10">
+        <v>38</v>
+      </c>
+      <c r="M5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="5">
         <v>33</v>
@@ -1368,11 +1437,14 @@
       <c r="I6" s="6">
         <v>40</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="13">
         <v>23</v>
       </c>
-      <c r="L6" s="7">
-        <v>45</v>
+      <c r="L6" s="11">
+        <v>32</v>
+      </c>
+      <c r="M6">
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1386,7 +1458,7 @@
       <c r="D7" s="6">
         <v>43</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>44</v>
       </c>
       <c r="F7" s="5">
@@ -1401,11 +1473,11 @@
       <c r="I7" s="6">
         <v>48</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="10">
         <v>24</v>
       </c>
-      <c r="L7">
-        <v>13</v>
+      <c r="L7" s="12">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1434,14 +1506,14 @@
       <c r="I8" s="5">
         <v>56</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="10">
         <v>26</v>
       </c>
       <c r="L8" s="8">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5">
         <v>57</v>
@@ -1467,14 +1539,14 @@
       <c r="I9" s="6">
         <v>64</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="11">
         <v>69</v>
       </c>
-      <c r="L9" s="10">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L9" s="12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="6">
         <v>65</v>
@@ -1494,17 +1566,17 @@
       <c r="G10" s="5">
         <v>70</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>71</v>
       </c>
       <c r="I10" s="6">
         <v>72</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="12">
         <v>33</v>
       </c>
-      <c r="L10" s="10">
-        <v>53</v>
+      <c r="L10" s="14">
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1524,7 +1596,7 @@
       <c r="F11" s="6">
         <v>77</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>78</v>
       </c>
       <c r="H11" s="6">
@@ -1533,86 +1605,86 @@
       <c r="I11" s="6">
         <v>80</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="12">
         <v>34</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K12" s="12">
+        <v>35</v>
+      </c>
+      <c r="L12" s="16">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K12" s="8">
-        <v>35</v>
-      </c>
-      <c r="L12" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="7">
+        <v>43</v>
+      </c>
+      <c r="K13" s="12">
+        <v>37</v>
+      </c>
+      <c r="L13" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K14" s="13">
+        <v>47</v>
+      </c>
+      <c r="L14" s="17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K15" s="10">
+        <v>62</v>
+      </c>
+      <c r="L15" s="14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K16" s="10">
+        <v>68</v>
+      </c>
+      <c r="L16" s="14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="11:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K17" s="11">
+        <v>70</v>
+      </c>
+      <c r="L17" s="14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="11:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K18" s="12">
+        <v>27</v>
+      </c>
+      <c r="L18" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K19" s="12">
+        <v>31</v>
+      </c>
+      <c r="L19" s="15">
         <v>16</v>
       </c>
-      <c r="K13" s="8">
-        <v>37</v>
-      </c>
-      <c r="L13" s="10">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K14" s="8">
-        <v>47</v>
-      </c>
-      <c r="L14" s="10">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K15" s="8">
-        <v>62</v>
-      </c>
-      <c r="L15" s="10">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K16" s="8">
-        <v>68</v>
-      </c>
-      <c r="L16" s="10">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K17" s="8">
-        <v>70</v>
-      </c>
-      <c r="L17" s="10">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K18" s="8">
-        <v>27</v>
-      </c>
-      <c r="L18" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K19" s="8">
-        <v>31</v>
-      </c>
-      <c r="L19" s="10">
+    </row>
+    <row r="20" spans="11:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K20" s="12">
+        <v>44</v>
+      </c>
+      <c r="L20" s="17">
         <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K20" s="8">
-        <v>46</v>
-      </c>
-      <c r="L20" s="10">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1622,10 +1694,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C199CFAC-6B78-4D74-875B-A9884636AB23}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1670,6 +1742,14 @@
       <c r="A6" t="s">
         <v>13</v>
       </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>